<commit_message>
merging with new 2 test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/input.xlsx
+++ b/src/test/resources/Data/input.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{E076A204-8B94-4DDD-8AC2-54CD3EF6DB62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{463A11F3-E7D8-41E9-AEF6-2850273EE873}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="17520" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="20760" windowHeight="11820" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TC01" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,12 @@
     <sheet name="TC04" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:Q23"/>
+  <oleSize ref="A1:S17"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>user name</t>
   </si>
@@ -30,9 +30,6 @@
     <t>admin</t>
   </si>
   <si>
-    <t>manager</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
@@ -69,15 +66,6 @@
     <t>Enter Title</t>
   </si>
   <si>
-    <t>actiTIME - Enter Time-Track</t>
-  </si>
-  <si>
-    <t>Version</t>
-  </si>
-  <si>
-    <t>actiTIME - Login</t>
-  </si>
-  <si>
     <t>45</t>
   </si>
   <si>
@@ -87,14 +75,26 @@
     <t>Build no</t>
   </si>
   <si>
-    <t>actiTIME 2019.Pro</t>
+    <t>rashmi@dell.com</t>
+  </si>
+  <si>
+    <t>Zoho CRM - Sign in</t>
+  </si>
+  <si>
+    <t>Zoho CRM - Home Page</t>
+  </si>
+  <si>
+    <t>campaign title</t>
+  </si>
+  <si>
+    <t>Zoho CRM - Create Campaign</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,6 +116,14 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -134,10 +142,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
@@ -145,8 +154,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -485,15 +496,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView zoomScale="77" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -505,24 +516,24 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
+      <c r="A2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="1">
+        <v>123456</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -530,8 +541,11 @@
       <c r="B3" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{6854BEE4-A169-48A8-A09B-A7D2967BB498}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -554,10 +568,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -565,42 +579,42 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -613,18 +627,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView zoomScale="77" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="77" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -650,7 +664,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -663,7 +677,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="4"/>

</xml_diff>

<commit_message>
after 2 test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/input.xlsx
+++ b/src/test/resources/Data/input.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{463A11F3-E7D8-41E9-AEF6-2850273EE873}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{596C1865-72F2-4A54-9C8B-4D8B75CFE19D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="20760" windowHeight="11820" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TC01" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,11 @@
     <sheet name="TC04" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:S17"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>user name</t>
   </si>
@@ -85,6 +84,9 @@
   </si>
   <si>
     <t>campaign title</t>
+  </si>
+  <si>
+    <t>123456</t>
   </si>
   <si>
     <t>Zoho CRM - Create Campaign</t>
@@ -497,18 +499,18 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView zoomScale="77" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -522,12 +524,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="1">
-        <v>123456</v>
+      <c r="B2" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
@@ -536,7 +538,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
     </row>
@@ -557,13 +559,13 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -574,7 +576,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -585,7 +587,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -593,7 +595,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -601,7 +603,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -609,7 +611,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -628,22 +630,22 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="77" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -657,12 +659,12 @@
   <sheetViews>
     <sheetView zoomScale="77" zoomScaleNormal="77" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>17</v>
       </c>
@@ -675,7 +677,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -687,7 +689,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="5"/>
       <c r="C3" s="4"/>

</xml_diff>

<commit_message>
update on tuesday 12-november at 2.27pm
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/input.xlsx
+++ b/src/test/resources/Data/input.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB5122B3-A3F6-44E0-87F9-93D78737ABE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{004A659A-854E-4325-AA41-57D078A093CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TC01" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>user name</t>
   </si>
@@ -96,6 +96,15 @@
   </si>
   <si>
     <t>Zoho CRM - Campaign Details</t>
+  </si>
+  <si>
+    <t>startdate</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>startcalendartitle</t>
   </si>
 </sst>
 </file>
@@ -154,7 +163,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
@@ -163,6 +172,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -508,15 +518,15 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -530,7 +540,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>16</v>
       </c>
@@ -544,7 +554,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
     </row>
@@ -565,13 +575,13 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -582,7 +592,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -593,7 +603,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -601,7 +611,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -609,7 +619,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -617,7 +627,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -636,20 +646,20 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView zoomScale="77" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -664,44 +674,55 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="C1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
+      <c r="C2" s="8">
+        <v>43811</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="5"/>
       <c r="C3" s="4"/>

</xml_diff>

<commit_message>
checking in on thurs 14-nov
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/input.xlsx
+++ b/src/test/resources/Data/input.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{004A659A-854E-4325-AA41-57D078A093CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BFFD02E-DE40-48F4-B200-4177E4FA5C8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>user name</t>
   </si>
@@ -105,6 +105,30 @@
   </si>
   <si>
     <t>startcalendartitle</t>
+  </si>
+  <si>
+    <t>Zoho CRM - Create Task</t>
+  </si>
+  <si>
+    <t>tasktitle</t>
+  </si>
+  <si>
+    <t>Highest</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>NEW TASK CREATED</t>
+  </si>
+  <si>
+    <t>lead/Contact</t>
+  </si>
+  <si>
+    <t>Leads</t>
   </si>
 </sst>
 </file>
@@ -674,7 +698,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,6 +707,7 @@
     <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -698,10 +723,18 @@
       <c r="D1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
+      <c r="E1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="I1" s="4"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -717,10 +750,18 @@
       <c r="D2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="E2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>

</xml_diff>

<commit_message>
added task and event
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/input.xlsx
+++ b/src/test/resources/Data/input.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{493D208D-64CC-4408-8373-0632D120BD2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E45D8C7-38D3-472A-B804-C9818EC7B98F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
   <si>
     <t>user name</t>
   </si>
@@ -137,10 +137,19 @@
     <t>Zoho CRM - Lead Name Lookup</t>
   </si>
   <si>
-    <t>getThisLead</t>
-  </si>
-  <si>
-    <t>sf sf</t>
+    <t>eventTitle</t>
+  </si>
+  <si>
+    <t>eventSubject</t>
+  </si>
+  <si>
+    <t>EVENT SUBJECT</t>
+  </si>
+  <si>
+    <t>Zoho CRM - Create Event</t>
+  </si>
+  <si>
+    <t>Event Time</t>
   </si>
 </sst>
 </file>
@@ -199,7 +208,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
@@ -209,6 +218,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -707,10 +717,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,9 +732,11 @@
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>22</v>
       </c>
@@ -755,8 +767,14 @@
       <c r="J1" s="4" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -785,10 +803,16 @@
         <v>38</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" s="9">
+        <v>0.46597222222222223</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="5"/>
       <c r="C3" s="4"/>

</xml_diff>

<commit_message>
nov-17- making generic methods for popup
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/input.xlsx
+++ b/src/test/resources/Data/input.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E45D8C7-38D3-472A-B804-C9818EC7B98F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{546E1E58-5125-4AC5-A2A6-448E533AA358}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
   <si>
     <t>user name</t>
   </si>
@@ -150,6 +150,12 @@
   </si>
   <si>
     <t>Event Time</t>
+  </si>
+  <si>
+    <t>SelectDropndown</t>
+  </si>
+  <si>
+    <t>Products</t>
   </si>
 </sst>
 </file>
@@ -717,10 +723,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,9 +740,10 @@
     <col min="9" max="9" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>22</v>
       </c>
@@ -773,8 +780,11 @@
       <c r="L1" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -811,8 +821,11 @@
       <c r="L2" s="9">
         <v>0.46597222222222223</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="5"/>
       <c r="C3" s="4"/>

</xml_diff>